<commit_message>
Add interactive column selection and export scripts
Introduces scripts for manual column selection and essential column export for HVAC dataset. Adds supporting JSON files for column selection progress and manual selections, updates dropped columns data, and extends allowed bash commands in settings.
</commit_message>
<xml_diff>
--- a/data/dropped_columns.xlsx
+++ b/data/dropped_columns.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MOIRAI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D1EEED-7B04-404B-A6EA-849CC5370859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10DAA4C-50D5-4580-9368-BA291034E133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="1530" windowWidth="16440" windowHeight="28320" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="no variation" sheetId="1" r:id="rId1"/>
     <sheet name="missing rate" sheetId="2" r:id="rId2"/>
+    <sheet name="tossed" sheetId="3" r:id="rId3"/>
+    <sheet name="essential" sheetId="4" r:id="rId4"/>
+    <sheet name="optional" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="197">
   <si>
     <t>column</t>
   </si>
@@ -106,6 +109,523 @@
   <si>
     <t>labview_Bedroom 3 Irradiance [W/m2]</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>egauge_Kitchen Lights [kW]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>egauge_H/Bd3/Bth2L [kW]</t>
+  </si>
+  <si>
+    <t>egauge_H/Bd3/Bth2L* [kVA]</t>
+  </si>
+  <si>
+    <t>egauge_Kitchen Lights* [kVA]</t>
+  </si>
+  <si>
+    <t>egauge_L1 Voltage [V]</t>
+  </si>
+  <si>
+    <t>egauge_L2 Voltage [V]</t>
+  </si>
+  <si>
+    <t>egauge_PBd/LR/Bd2L [kW]</t>
+  </si>
+  <si>
+    <t>egauge_PBd/LR/Bd2L* [kVA]</t>
+  </si>
+  <si>
+    <t>egauge_PBth/UtlL [kW]</t>
+  </si>
+  <si>
+    <t>egauge_PBth/UtlL* [kVA]</t>
+  </si>
+  <si>
+    <t>egauge_Test Voltage [V]</t>
+  </si>
+  <si>
+    <t>egauge_Water Heater [kW]</t>
+  </si>
+  <si>
+    <t>egauge_Water Heater* [kVA]</t>
+  </si>
+  <si>
+    <t>labview_A_Bot [V]</t>
+  </si>
+  <si>
+    <t>labview_A_Bot_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_A_Top [V]</t>
+  </si>
+  <si>
+    <t>labview_A_Top_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_BGlobe</t>
+  </si>
+  <si>
+    <t>labview_B_Bot [V]</t>
+  </si>
+  <si>
+    <t>labview_B_Top [V]</t>
+  </si>
+  <si>
+    <t>labview_Bedroom 2 Pyranometer Irradiance [W/m2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labview_Bedroom 2 Pyranometer [V] </t>
+  </si>
+  <si>
+    <t>labview_Bedroom 3 Irradiance [W/m2]</t>
+  </si>
+  <si>
+    <t>labview_Bedroom 3 Pyranometer Irradiance [W/m2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labview_Bedroom 3 Pyranometer [V] </t>
+  </si>
+  <si>
+    <t>labview_C_Bot [V]</t>
+  </si>
+  <si>
+    <t>labview_C_Top [V]</t>
+  </si>
+  <si>
+    <t>labview_D_Bot [V]</t>
+  </si>
+  <si>
+    <t>labview_D_Top [V]</t>
+  </si>
+  <si>
+    <t>labview_E_Bot [V]</t>
+  </si>
+  <si>
+    <t>labview_E_Top [V]</t>
+  </si>
+  <si>
+    <t>labview_F_Bot [V]</t>
+  </si>
+  <si>
+    <t>labview_F_Top [V]</t>
+  </si>
+  <si>
+    <t>labview_G_Bot[V]</t>
+  </si>
+  <si>
+    <t>labview_G_Top [V]</t>
+  </si>
+  <si>
+    <t>labview_H_Bot [V]</t>
+  </si>
+  <si>
+    <t>labview_H_Top [V]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labview_Kitchen Pyranometer Irradiance [W/m2] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">labview_Kitchen Pyranometer [V] </t>
+  </si>
+  <si>
+    <t>labview_Living Room Pyranometer Irradiance [W/m2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labview_Living Room Pyranometer [V] </t>
+  </si>
+  <si>
+    <t>labview_Master Bedroom Pyranometer Irradiance [W/m2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labview_Master Bedroom Pyranometer [V] </t>
+  </si>
+  <si>
+    <t>labview_ODU Coil3</t>
+  </si>
+  <si>
+    <t>labview_ODU CoilIn</t>
+  </si>
+  <si>
+    <t>labview_ODU CoilInt</t>
+  </si>
+  <si>
+    <t>labview_ODU CoilOut</t>
+  </si>
+  <si>
+    <t>labview_ODU CompDis</t>
+  </si>
+  <si>
+    <t>labview_ODU CompSuc</t>
+  </si>
+  <si>
+    <t>labview_ODU off</t>
+  </si>
+  <si>
+    <t>labview_Wind Measurement Quality [%]</t>
+  </si>
+  <si>
+    <t>egauge_Indoor Unit Extra [kW]</t>
+  </si>
+  <si>
+    <t>egauge_Indoor Unit Extra* [kVA]</t>
+  </si>
+  <si>
+    <t>egauge_Indoor Unit [kW]</t>
+  </si>
+  <si>
+    <t>egauge_Indoor Unit* [kVA]</t>
+  </si>
+  <si>
+    <t>egauge_Main Power [kW]</t>
+  </si>
+  <si>
+    <t>egauge_Main Power* [kVA]</t>
+  </si>
+  <si>
+    <t>egauge_Outdoor Unit [kW]</t>
+  </si>
+  <si>
+    <t>egauge_Outdoor Unit* [kVA]</t>
+  </si>
+  <si>
+    <t>egauge_S1 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S10 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S11 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S12 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S13 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S14 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S2 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S3 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S4 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S5 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S6 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S7 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S8 [A]</t>
+  </si>
+  <si>
+    <t>egauge_S9 [A]</t>
+  </si>
+  <si>
+    <t>labview_A1</t>
+  </si>
+  <si>
+    <t>labview_A2</t>
+  </si>
+  <si>
+    <t>labview_A3</t>
+  </si>
+  <si>
+    <t>labview_A5</t>
+  </si>
+  <si>
+    <t>labview_A6</t>
+  </si>
+  <si>
+    <t>labview_A7</t>
+  </si>
+  <si>
+    <t>labview_Air Temperature [degC]</t>
+  </si>
+  <si>
+    <t>labview_B1</t>
+  </si>
+  <si>
+    <t>labview_B2</t>
+  </si>
+  <si>
+    <t>labview_B3</t>
+  </si>
+  <si>
+    <t>labview_B5</t>
+  </si>
+  <si>
+    <t>labview_B6</t>
+  </si>
+  <si>
+    <t>labview_B7</t>
+  </si>
+  <si>
+    <t>labview_B_Bot_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_B_Top_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_C1</t>
+  </si>
+  <si>
+    <t>labview_C2</t>
+  </si>
+  <si>
+    <t>labview_C3</t>
+  </si>
+  <si>
+    <t>labview_C5</t>
+  </si>
+  <si>
+    <t>labview_C6</t>
+  </si>
+  <si>
+    <t>labview_C7</t>
+  </si>
+  <si>
+    <t>labview_CO2 [ppm]</t>
+  </si>
+  <si>
+    <t>labview_C_Bot_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_C_Top_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_D1</t>
+  </si>
+  <si>
+    <t>labview_D2</t>
+  </si>
+  <si>
+    <t>labview_D3</t>
+  </si>
+  <si>
+    <t>labview_D5</t>
+  </si>
+  <si>
+    <t>labview_D6</t>
+  </si>
+  <si>
+    <t>labview_D7</t>
+  </si>
+  <si>
+    <t>labview_D_Bot_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_D_Top_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_Dew Point [degC]</t>
+  </si>
+  <si>
+    <t>labview_E1</t>
+  </si>
+  <si>
+    <t>labview_E2</t>
+  </si>
+  <si>
+    <t>labview_E3</t>
+  </si>
+  <si>
+    <t>labview_E5</t>
+  </si>
+  <si>
+    <t>labview_E6</t>
+  </si>
+  <si>
+    <t>labview_E7</t>
+  </si>
+  <si>
+    <t>labview_E_Bot_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_E_Top_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_F1</t>
+  </si>
+  <si>
+    <t>labview_F2</t>
+  </si>
+  <si>
+    <t>labview_F3</t>
+  </si>
+  <si>
+    <t>labview_F5</t>
+  </si>
+  <si>
+    <t>labview_F6</t>
+  </si>
+  <si>
+    <t>labview_F7</t>
+  </si>
+  <si>
+    <t>labview_F_Bot_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_F_Top_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_G1</t>
+  </si>
+  <si>
+    <t>labview_G2</t>
+  </si>
+  <si>
+    <t>labview_G3</t>
+  </si>
+  <si>
+    <t>labview_G5</t>
+  </si>
+  <si>
+    <t>labview_G6</t>
+  </si>
+  <si>
+    <t>labview_G7</t>
+  </si>
+  <si>
+    <t>labview_G_Bot_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_G_Top_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_H1</t>
+  </si>
+  <si>
+    <t>labview_H2</t>
+  </si>
+  <si>
+    <t>labview_H3</t>
+  </si>
+  <si>
+    <t>labview_H5</t>
+  </si>
+  <si>
+    <t>labview_H6</t>
+  </si>
+  <si>
+    <t>labview_H7</t>
+  </si>
+  <si>
+    <t>labview_H_Bot_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_H_Top_HF [W/m^2]</t>
+  </si>
+  <si>
+    <t>labview_IDU CoilIn</t>
+  </si>
+  <si>
+    <t>labview_IDU CoilInt</t>
+  </si>
+  <si>
+    <t>labview_IDU Distributor</t>
+  </si>
+  <si>
+    <t>labview_IDU Return Air</t>
+  </si>
+  <si>
+    <t>labview_Precipitation Type</t>
+  </si>
+  <si>
+    <t>labview_Relative Air Pressure [kPa]</t>
+  </si>
+  <si>
+    <t>labview_Relative Humidity [%]</t>
+  </si>
+  <si>
+    <t>labview_Return RH[%]</t>
+  </si>
+  <si>
+    <t>labview_SV1</t>
+  </si>
+  <si>
+    <t>labview_SV2</t>
+  </si>
+  <si>
+    <t>labview_SV2 New</t>
+  </si>
+  <si>
+    <t>labview_SV3 New</t>
+  </si>
+  <si>
+    <t>labview_SV4</t>
+  </si>
+  <si>
+    <t>labview_SV5</t>
+  </si>
+  <si>
+    <t>labview_SV6</t>
+  </si>
+  <si>
+    <t>labview_TVOC[ug/m3]</t>
+  </si>
+  <si>
+    <t>labview_Thermostat</t>
+  </si>
+  <si>
+    <t>labview_TstatRH [%]</t>
+  </si>
+  <si>
+    <t>labview_Wind Chill Temperature [degC]</t>
+  </si>
+  <si>
+    <t>labview_Wind Direction [deg]</t>
+  </si>
+  <si>
+    <t>labview_Wind Speed [m/s]</t>
+  </si>
+  <si>
+    <t>labview_BR1-SV1 RH [%]</t>
+  </si>
+  <si>
+    <t>labview_BR3 SV RH [%]</t>
+  </si>
+  <si>
+    <t>labview_BTH SV RH [%]</t>
+  </si>
+  <si>
+    <t>labview_Bath2 SV</t>
+  </si>
+  <si>
+    <t>labview_ODU Coil2</t>
+  </si>
+  <si>
+    <t>labview_SV1 RH [%]</t>
+  </si>
+  <si>
+    <t>labview_SV2 RH [%]</t>
+  </si>
+  <si>
+    <t>labview_SV3 RH[%]</t>
+  </si>
+  <si>
+    <t>labview_MB RH [%]</t>
+  </si>
+  <si>
+    <t>labview_BR1 SV2 RH [%]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>labview_BR3 RH [%]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>labview_IDU CoilOut</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -653,7 +1173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF0A5DF-D3C3-4A9D-8B86-2BB322671BAC}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -789,4 +1309,977 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48610DC9-00DA-4108-B0CA-B453CBE8EB1D}">
+  <dimension ref="A1:A61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="47.46484375" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEE03EC-545D-4EFB-B818-6BE09D8EC1B7}">
+  <dimension ref="A1:A112"/>
+  <sheetViews>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="31.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A98" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A101" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A107" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC368138-93F3-43B0-A849-061F30EE2A41}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>